<commit_message>
adjust connection with categories table
</commit_message>
<xml_diff>
--- a/Database/database-concept.xlsx
+++ b/Database/database-concept.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Iskolai fejlesztés\Projekt\Anyaközösség projekt\Database-structure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Ágazati vizsga projekt\anyakozosseg-backend\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AD5D83-66EB-429E-B033-9A764CC0BE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-111" yWindow="-111" windowWidth="23254" windowHeight="12574"/>
   </bookViews>
   <sheets>
     <sheet name="Database Structure" sheetId="1" r:id="rId1"/>
-    <sheet name="Example of table contents" sheetId="3" r:id="rId2"/>
+    <sheet name="Munka1" sheetId="4" r:id="rId2"/>
+    <sheet name="Example of table contents" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -146,12 +146,24 @@
   </si>
   <si>
     <t>image_path</t>
+  </si>
+  <si>
+    <t>categories_to_ingredients</t>
+  </si>
+  <si>
+    <t>categories_to_products</t>
+  </si>
+  <si>
+    <t>categories_to_brands</t>
+  </si>
+  <si>
+    <t>brand_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -220,36 +232,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -404,98 +386,92 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,168 +494,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>242835</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>87923</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>456362</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>87923</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="49" name="Egyenes összekötő 48">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2482780" y="3801626"/>
-          <a:ext cx="213527" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>248697</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>117230</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>248697</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="Egyenes összekötő 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2118200" y="2616212"/>
-          <a:ext cx="0" cy="4071403"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>244929</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>124688</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>502418</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>124688</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="55" name="Egyenes összekötő 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2114432" y="6679781"/>
-          <a:ext cx="257489" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>66990</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>83736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>213528</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>83736</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -722,15 +545,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217715</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>106032</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217715</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>120118</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -773,13 +596,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>83737</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>108859</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>213528</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>108859</xdr:rowOff>
@@ -824,15 +647,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217715</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>99392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217715</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>113659</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -875,15 +698,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>104671</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>385187</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>104671</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -928,15 +751,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>226088</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>121418</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>385187</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>121418</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -981,15 +804,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>41868</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>85244</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>221901</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>85244</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1032,15 +855,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>93044</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1083,15 +906,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>100483</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>418681</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>100483</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1136,67 +959,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>235404</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>118530</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>59683</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>99662</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>480473</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>118530</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="83" name="Egyenes összekötő 82">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2102304" y="2638573"/>
-          <a:ext cx="245069" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>48798</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>105104</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>251498</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>105104</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>473529</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>99662</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1211,8 +983,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1914384" y="2229695"/>
-          <a:ext cx="202700" cy="0"/>
+          <a:off x="4468397" y="3980419"/>
+          <a:ext cx="413846" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1240,13 +1012,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>80460</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>104124</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>373900</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>104124</xdr:rowOff>
@@ -1293,13 +1065,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>105456</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>374196</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>105456</xdr:rowOff>
@@ -1346,15 +1118,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>41291</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>97823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>187829</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>97823</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1397,15 +1169,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>192016</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>97596</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>192016</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>107394</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1448,15 +1220,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>185149</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>109227</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>344248</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>109227</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1501,15 +1273,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>209308</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>125347</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>368407</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>125347</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1534,6 +1306,373 @@
         <a:ln w="28575">
           <a:tailEnd type="triangle"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>48797</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>94218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>462643</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>94218</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Egyenes összekötő nyíllal 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4457511" y="6130347"/>
+          <a:ext cx="413846" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>48797</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>94219</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>462643</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>94219</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Egyenes összekötő nyíllal 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4457511" y="2418319"/>
+          <a:ext cx="413846" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>234042</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>87087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>234042</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>125185</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Egyenes összekötő 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2400299" y="2607130"/>
+          <a:ext cx="0" cy="3739241"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>224413</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>99227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>425380</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>99227</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Egyenes összekötő nyíllal 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2390670" y="2619270"/>
+          <a:ext cx="200967" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>429568</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Egyenes összekötő nyíllal 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2394858" y="4370615"/>
+          <a:ext cx="200967" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>223158</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>424125</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Egyenes összekötő nyíllal 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2389415" y="6340929"/>
+          <a:ext cx="200967" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>86148</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>98386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>232686</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>98386</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Egyenes összekötő 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000072000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2252405" y="4371029"/>
+          <a:ext cx="146538" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -1817,399 +1956,429 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.21875" style="9"/>
+    <col min="1" max="1" width="3.53515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.921875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12.15234375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.84375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.15234375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="7.765625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="17.3046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.07421875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.07421875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="19.84375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.07421875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.23046875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="26" t="s">
+    <row r="1" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="10" t="s">
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="12" t="s">
+    <row r="4" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="H4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E5" s="13" t="s">
+    <row r="5" spans="5:12" x14ac:dyDescent="0.4">
+      <c r="H5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="14" t="s">
+    <row r="6" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="26" t="s">
+    <row r="7" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="H8" s="26" t="s">
+      <c r="I8" s="29"/>
+      <c r="K8" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="10" t="s">
+      <c r="L8" s="29"/>
+    </row>
+    <row r="9" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="K9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="L9" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E10" s="5" t="s">
+    <row r="10" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="K10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="L10" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E12" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="29"/>
+      <c r="H12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="10" t="s">
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="26" t="s">
+    <row r="14" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E14" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="H15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="29"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="K19" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H20" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E21" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="29"/>
+      <c r="H21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" s="27"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="E14" s="21" t="s">
+      <c r="C22" s="29"/>
+      <c r="E22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F23" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23" s="20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="10" t="s">
+      <c r="H24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H27" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H28" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="I28" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="K28" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="27"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="K30" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="L30" s="23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
+    <row r="31" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E31" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="H31" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="27"/>
+    </row>
+    <row r="32" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E32" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E33" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="I33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="4" t="s">
+    </row>
+    <row r="34" spans="5:9" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="H34" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="I18" s="27"/>
-    </row>
-    <row r="19" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H20" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="29"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="I23" s="27"/>
-    </row>
-    <row r="24" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E29" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="29"/>
-    </row>
-    <row r="30" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E30" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30" s="29"/>
-    </row>
-    <row r="31" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E31" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H32" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E33" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="29"/>
-    </row>
-    <row r="34" spans="5:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E34" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E37" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E38" s="3" t="s">
+    <row r="35" spans="5:9" x14ac:dyDescent="0.4">
+      <c r="H35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E39" s="3" t="s">
+    <row r="36" spans="5:9" x14ac:dyDescent="0.4">
+      <c r="H36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="5:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E40" s="5" t="s">
+    <row r="37" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="I37" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="5:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="5:9" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="11">
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H30:I30"/>
+  <mergeCells count="14">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2218,27 +2387,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.69140625" customWidth="1"/>
+    <col min="3" max="3" width="18.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="27"/>
-    </row>
-    <row r="3" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="29"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="8" t="s">
         <v>22</v>
       </c>
@@ -2247,7 +2430,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -2255,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -2263,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -2271,7 +2454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B7" s="3">
         <v>2</v>
       </c>
@@ -2279,7 +2462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -2287,7 +2470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B9" s="3">
         <v>2</v>
       </c>
@@ -2295,7 +2478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B10" s="3">
         <v>2</v>
       </c>
@@ -2303,7 +2486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B11" s="3">
         <v>3</v>
       </c>
@@ -2311,7 +2494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B12" s="3">
         <v>3</v>
       </c>
@@ -2319,7 +2502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B13" s="3">
         <v>3</v>
       </c>
@@ -2327,7 +2510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="5">
         <v>3</v>
       </c>
@@ -2335,7 +2518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>

</xml_diff>

<commit_message>
add ratings table to the database
</commit_message>
<xml_diff>
--- a/Database/database-concept.xlsx
+++ b/Database/database-concept.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -158,6 +158,21 @@
   </si>
   <si>
     <t>brand_id</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>ratings</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>int(5)</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -461,16 +476,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -671,8 +686,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4560795" y="1833102"/>
-          <a:ext cx="0" cy="1771990"/>
+          <a:off x="6841672" y="1835663"/>
+          <a:ext cx="0" cy="1570925"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1662,6 +1677,157 @@
           <a:ext cx="402769" cy="179614"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>97970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>468087</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>97970</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Szögletes összekötő 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="4136572" y="484413"/>
+          <a:ext cx="429986" cy="195943"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>244930</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>77620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>244930</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>97331</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Egyenes összekötő 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4343401" y="850506"/>
+          <a:ext cx="0" cy="1570925"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>30325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>258925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Egyenes összekötő nyíllal 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4132684" y="847531"/>
+          <a:ext cx="228600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
@@ -1953,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1976,12 +2142,22 @@
   <sheetData>
     <row r="1" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H2" s="28" t="s">
+      <c r="E2" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="H2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>1</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>0</v>
       </c>
@@ -1990,6 +2166,12 @@
       </c>
     </row>
     <row r="4" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="E4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="H4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1998,6 +2180,12 @@
       </c>
     </row>
     <row r="5" spans="5:12" x14ac:dyDescent="0.4">
+      <c r="E5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H5" s="13" t="s">
         <v>3</v>
       </c>
@@ -2006,6 +2194,12 @@
       </c>
     </row>
     <row r="6" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="H6" s="14" t="s">
         <v>4</v>
       </c>
@@ -2014,18 +2208,24 @@
       </c>
     </row>
     <row r="7" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
     </row>
     <row r="8" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="K8" s="28" t="s">
+      <c r="I8" s="27"/>
+      <c r="K8" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="29"/>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H9" s="10" t="s">
@@ -2057,14 +2257,14 @@
     </row>
     <row r="11" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="12" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="H12" s="26" t="s">
+      <c r="F12" s="27"/>
+      <c r="H12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="27"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E13" s="17" t="s">
@@ -2117,10 +2317,10 @@
       <c r="I17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="L17" s="29"/>
+      <c r="L17" s="27"/>
     </row>
     <row r="18" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H18" s="5" t="s">
@@ -2145,32 +2345,32 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="27"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="29"/>
+      <c r="F21" s="27"/>
       <c r="H21" s="10" t="s">
         <v>0</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="K21" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="L21" s="27"/>
+      <c r="L21" s="29"/>
     </row>
     <row r="22" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="29"/>
+      <c r="C22" s="27"/>
       <c r="E22" s="17" t="s">
         <v>32</v>
       </c>
@@ -2246,10 +2446,10 @@
     </row>
     <row r="26" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="27" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H27" s="26" t="s">
+      <c r="H27" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="27"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H28" s="10" t="s">
@@ -2258,10 +2458,10 @@
       <c r="I28" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K28" s="26" t="s">
+      <c r="K28" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="27"/>
+      <c r="L28" s="29"/>
     </row>
     <row r="29" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H29" s="5" t="s">
@@ -2286,14 +2486,14 @@
       </c>
     </row>
     <row r="31" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="27"/>
-      <c r="H31" s="26" t="s">
+      <c r="F31" s="29"/>
+      <c r="H31" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="27"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E32" s="17" t="s">
@@ -2366,7 +2566,15 @@
     <row r="39" spans="5:9" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="K8:L8"/>
@@ -2374,13 +2582,6 @@
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2418,10 +2619,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="29"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" spans="2:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="8" t="s">

</xml_diff>

<commit_message>
extend ratings database table with a timestamp
</commit_message>
<xml_diff>
--- a/Database/database-concept.xlsx
+++ b/Database/database-concept.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>added_on</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -476,16 +482,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2120,7 +2126,7 @@
   <dimension ref="B1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2142,14 +2148,14 @@
   <sheetData>
     <row r="1" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="H2" s="26" t="s">
+      <c r="F2" s="29"/>
+      <c r="H2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="27"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E3" s="10" t="s">
@@ -2208,24 +2214,30 @@
       </c>
     </row>
     <row r="7" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="16"/>
     </row>
     <row r="8" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H8" s="26" t="s">
+      <c r="E8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="27"/>
-      <c r="K8" s="26" t="s">
+      <c r="I8" s="29"/>
+      <c r="K8" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="27"/>
+      <c r="L8" s="29"/>
     </row>
     <row r="9" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H9" s="10" t="s">
@@ -2257,14 +2269,14 @@
     </row>
     <row r="11" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="12" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="H12" s="28" t="s">
+      <c r="F12" s="29"/>
+      <c r="H12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="29"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="5:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E13" s="17" t="s">
@@ -2317,10 +2329,10 @@
       <c r="I17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="L17" s="27"/>
+      <c r="L17" s="29"/>
     </row>
     <row r="18" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H18" s="5" t="s">
@@ -2345,32 +2357,32 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="29"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="27"/>
+      <c r="F21" s="29"/>
       <c r="H21" s="10" t="s">
         <v>0</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L21" s="29"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="29"/>
       <c r="E22" s="17" t="s">
         <v>32</v>
       </c>
@@ -2446,10 +2458,10 @@
     </row>
     <row r="26" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="27" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H27" s="28" t="s">
+      <c r="H27" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="29"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H28" s="10" t="s">
@@ -2458,10 +2470,10 @@
       <c r="I28" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K28" s="28" t="s">
+      <c r="K28" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="29"/>
+      <c r="L28" s="27"/>
     </row>
     <row r="29" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="H29" s="5" t="s">
@@ -2486,14 +2498,14 @@
       </c>
     </row>
     <row r="31" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="H31" s="28" t="s">
+      <c r="F31" s="27"/>
+      <c r="H31" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="29"/>
+      <c r="I31" s="27"/>
     </row>
     <row r="32" spans="2:12" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E32" s="17" t="s">
@@ -2567,6 +2579,13 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="15">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E12:F12"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="H2:I2"/>
@@ -2575,13 +2594,6 @@
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2619,10 +2631,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="2:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="8" t="s">

</xml_diff>